<commit_message>
Solid state eem correction performed
@maggiebowman6 still need to put plots onto one page, but for now here is some raw output to look thru before our meeting.

Check for corrected eems in Fluoro-Package/ 180316/corrected, and plots in the plots folder within the corrected folder.
</commit_message>
<xml_diff>
--- a/F4SPF_LOG SHEET_BBWM_180426.xlsx
+++ b/F4SPF_LOG SHEET_BBWM_180426.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maggi\Desktop\180316\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rlee/Dropbox/GitHub/Fluoro-Package/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{47E10A17-2B25-3240-AA33-CA322D776629}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="12720" yWindow="460" windowWidth="15500" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="76">
   <si>
     <t>Name of Raw EEM</t>
   </si>
@@ -48,18 +48,6 @@
     <t>BBWMO120X</t>
   </si>
   <si>
-    <t>BBWMO1181</t>
-  </si>
-  <si>
-    <t>BBWMO118110X</t>
-  </si>
-  <si>
-    <t>BBWMO118120X</t>
-  </si>
-  <si>
-    <t>BBWMO118140X</t>
-  </si>
-  <si>
     <t>combBBWMO1</t>
   </si>
   <si>
@@ -250,12 +238,27 @@
   </si>
   <si>
     <t>COMBNaCO3NKSMPLHLDRBBWMO118140X</t>
+  </si>
+  <si>
+    <t>BBWMO181</t>
+  </si>
+  <si>
+    <t>BBWMO18120X</t>
+  </si>
+  <si>
+    <t>BBWMO18140X</t>
+  </si>
+  <si>
+    <t>BBWMO18110X</t>
+  </si>
+  <si>
+    <t>COMBSMPLHLDRBBWM0181</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,23 +603,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -630,721 +633,721 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
         <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
       </c>
       <c r="D18">
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
         <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D21">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
         <v>47</v>
-      </c>
-      <c r="C25" t="s">
-        <v>51</v>
       </c>
       <c r="D25">
         <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D27">
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D28">
         <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D29">
         <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D31">
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D32">
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D34">
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D35">
         <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D36">
         <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D38">
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D39">
         <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D41">
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D42">
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D43">
         <v>40</v>
       </c>
       <c r="E43" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>